<commit_message>
hoan thanh form thực hành chương 1
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources1/Du lieu cau hoi/thu vien bai hoc.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources1/Du lieu cau hoi/thu vien bai hoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Dang_Quy_UTE_k19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources1\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04065A3B-400A-4972-94A4-E7018C4ED49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259B9A23-4F01-44E1-9E82-DFE3F8AC8599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2871" uniqueCount="671">
   <si>
     <t>nActi</t>
   </si>
@@ -2742,6 +2742,9 @@
   </si>
   <si>
     <t>box</t>
+  </si>
+  <si>
+    <t>dien</t>
   </si>
 </sst>
 </file>
@@ -3303,10 +3306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3321,7 +3324,7 @@
     <col min="12" max="16384" width="12.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3359,10 +3362,13 @@
         <v>592</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="207.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="207.6" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
@@ -3402,8 +3408,11 @@
       <c r="M2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="83.4" x14ac:dyDescent="0.3">
+      <c r="N2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="83.4" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -3441,10 +3450,13 @@
         <v>14</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="55.8" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>18</v>
       </c>
@@ -3484,8 +3496,11 @@
       <c r="M4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="N4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
@@ -3523,10 +3538,13 @@
         <v>14</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>20</v>
       </c>
@@ -3566,8 +3584,11 @@
       <c r="M6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="83.4" x14ac:dyDescent="0.3">
+      <c r="N6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="83.4" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>21</v>
       </c>
@@ -3607,8 +3628,11 @@
       <c r="M7" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="N7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>22</v>
       </c>
@@ -3648,8 +3672,11 @@
       <c r="M8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+      <c r="N8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -3689,8 +3716,11 @@
       <c r="M9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="N9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>24</v>
       </c>
@@ -3730,8 +3760,11 @@
       <c r="M10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -3771,8 +3804,11 @@
       <c r="M11" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="N11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>26</v>
       </c>
@@ -3813,7 +3849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>29</v>
       </c>
@@ -3853,8 +3889,11 @@
       <c r="M13" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="N13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>30</v>
       </c>
@@ -3894,8 +3933,11 @@
       <c r="M14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="N14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>31</v>
       </c>
@@ -3935,8 +3977,11 @@
       <c r="M15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="83.4" x14ac:dyDescent="0.3">
+      <c r="N15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="83.4" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>32</v>
       </c>
@@ -3976,8 +4021,11 @@
       <c r="M16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="N16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>33</v>
       </c>
@@ -4017,8 +4065,11 @@
       <c r="M17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -9373,10 +9424,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9387,7 +9438,7 @@
     <col min="5" max="16384" width="12.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -9428,10 +9479,13 @@
         <v>592</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="83.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="83.4" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
@@ -9474,8 +9528,11 @@
       <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -9518,8 +9575,11 @@
       <c r="N3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="O3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>18</v>
       </c>
@@ -9562,8 +9622,11 @@
       <c r="N4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="O4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
@@ -9606,8 +9669,11 @@
       <c r="N5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="O5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>20</v>
       </c>
@@ -9650,8 +9716,11 @@
       <c r="N6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="O6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>21</v>
       </c>
@@ -9694,8 +9763,11 @@
       <c r="N7" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="O7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>22</v>
       </c>
@@ -9738,8 +9810,11 @@
       <c r="N8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="42" x14ac:dyDescent="0.3">
+      <c r="O8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -9782,8 +9857,11 @@
       <c r="N9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="O9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>24</v>
       </c>
@@ -9826,8 +9904,11 @@
       <c r="N10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="O10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -9870,8 +9951,11 @@
       <c r="N11" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="O11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>26</v>
       </c>
@@ -9914,8 +9998,11 @@
       <c r="N12" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="42" x14ac:dyDescent="0.3">
+      <c r="O12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="42" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>29</v>
       </c>
@@ -9958,8 +10045,11 @@
       <c r="N13" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>28</v>
       </c>

</xml_diff>